<commit_message>
Excel and pbix file changes are committed
</commit_message>
<xml_diff>
--- a/Data Insights.xlsx
+++ b/Data Insights.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAVI\Interview Preparation\Personal Projects\Power BI Projects\Global_Store_Data_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7A2433-03C6-497B-B10A-B866B4D35DAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109BE845-E1A9-47E6-86E4-32D2CFAD84B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Insights" sheetId="1" r:id="rId1"/>
+    <sheet name="Measures" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Data Insights</t>
   </si>
@@ -46,6 +47,99 @@
   </si>
   <si>
     <t>Consumer products have the most sales</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phones are most bought sub category </t>
+  </si>
+  <si>
+    <t>Report Name</t>
+  </si>
+  <si>
+    <t>Sales Analysis</t>
+  </si>
+  <si>
+    <t>Profit Analysis</t>
+  </si>
+  <si>
+    <t>Technology products are most profitable category</t>
+  </si>
+  <si>
+    <t>Copiers are most profitable sub category</t>
+  </si>
+  <si>
+    <t>Global store sales are most profitable in United States</t>
+  </si>
+  <si>
+    <t>State where sales are most profitable is in England, next is California</t>
+  </si>
+  <si>
+    <t>Sales are most profitable in New york city</t>
+  </si>
+  <si>
+    <t>Australia and France have most sales than China but China is more profitable than them. Need to investigate why ?</t>
+  </si>
+  <si>
+    <t>India and UK have less sales comparatively but are in top 4 in terms of profits. Need to investigate why ?</t>
+  </si>
+  <si>
+    <t>Manila city has good sales but profits are less, need to investigate ?</t>
+  </si>
+  <si>
+    <t>Europe market is highly profitable and next is Asia pacific</t>
+  </si>
+  <si>
+    <t>Most sales are recorded in Western Europe region followed by Central America</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>DAX Calculation</t>
+  </si>
+  <si>
+    <t>% of Sales by Region</t>
+  </si>
+  <si>
+    <t>Total Sales</t>
+  </si>
+  <si>
+    <t>SUM(Orders[Sales])</t>
+  </si>
+  <si>
+    <t>Total Profit</t>
+  </si>
+  <si>
+    <t>SUM(Orders[Profit])</t>
+  </si>
+  <si>
+    <t>Total Shipping Cost</t>
+  </si>
+  <si>
+    <t>SUM(Orders[Shipping Cost])</t>
+  </si>
+  <si>
+    <t>Total Customers</t>
+  </si>
+  <si>
+    <t>DISTINCTCOUNT(Orders[Customer ID])</t>
+  </si>
+  <si>
+    <t>Total Orders</t>
+  </si>
+  <si>
+    <t>DISTINCTCOUNT(Orders[Order ID])</t>
+  </si>
+  <si>
+    <t>DIVIDE([TotalSales], CALCULATE(SUM(Orders[Sales]), ALL(Orders[Region]))) * 100</t>
+  </si>
+  <si>
+    <t>Western Africa, Central Asia and Western Asia have negative profits</t>
+  </si>
+  <si>
+    <t>DIVIDE([TotalProfit], CALCULATE(SUM(Orders[Profit]), ALL(Orders[Region]))) * 100</t>
+  </si>
+  <si>
+    <t>% of Profits By Region</t>
   </si>
 </sst>
 </file>
@@ -395,50 +489,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="72.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="95.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B4EEEFE-DE7A-4A9F-BC63-B4364F57AC98}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="86" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Sales and Profit by Year and Drill through functionality
</commit_message>
<xml_diff>
--- a/Data Insights.xlsx
+++ b/Data Insights.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RAVI\Interview Preparation\Personal Projects\Power BI Projects\Global_Store_Data_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{109BE845-E1A9-47E6-86E4-32D2CFAD84B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8E67D83-CD51-49FD-A5D6-2CB2905427AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Data Insights</t>
   </si>
@@ -140,6 +140,9 @@
   </si>
   <si>
     <t>% of Profits By Region</t>
+  </si>
+  <si>
+    <t>In 2015 Quarter 4, there is a discrepancy, December_Sales &gt; October_Sales but December_Profit &lt; October_Profit. Need to investigate.</t>
   </si>
 </sst>
 </file>
@@ -489,16 +492,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="95.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="121.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -552,56 +555,61 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>